<commit_message>
renaming and updating things
</commit_message>
<xml_diff>
--- a/src/compiler/data/XAIP.xlsx
+++ b/src/compiler/data/XAIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarathsreedharan/mycode/survey-visualizer/src/compiler/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{811D2AE8-49EC-E643-A5DA-29DF39F0DB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E0AF383-4255-3346-B463-86F29CEEA9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -83,9 +83,6 @@
   </si>
   <si>
     <t>HTN</t>
-  </si>
-  <si>
-    <t>FOND</t>
   </si>
   <si>
     <t>Partial Observability</t>
@@ -636,6 +633,9 @@
   </si>
   <si>
     <t>Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>Qualitative Non-Determinism</t>
   </si>
 </sst>
 </file>
@@ -1577,8 +1577,8 @@
   <dimension ref="A1:EZ274"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y3" sqref="Y3"/>
+      <pane ySplit="6" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1600,7 +1600,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="115" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F1" s="116"/>
       <c r="G1" s="116"/>
@@ -1613,10 +1613,10 @@
       <c r="N1" s="116"/>
       <c r="O1" s="116"/>
       <c r="P1" s="108" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="115" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="R1" s="116"/>
       <c r="S1" s="116"/>
@@ -1627,7 +1627,7 @@
       <c r="X1" s="116"/>
       <c r="Y1" s="116"/>
       <c r="Z1" s="115" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AA1" s="116"/>
       <c r="AB1" s="116"/>
@@ -1638,17 +1638,17 @@
     </row>
     <row r="2" spans="1:156" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="E2" s="115" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F2" s="116"/>
       <c r="G2" s="116"/>
       <c r="H2" s="116"/>
       <c r="I2" s="115" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J2" s="116"/>
       <c r="K2" s="115" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L2" s="116"/>
       <c r="M2" s="116"/>
@@ -1662,16 +1662,16 @@
         <v>16</v>
       </c>
       <c r="Q2" s="108" t="s">
+        <v>200</v>
+      </c>
+      <c r="R2" s="108" t="s">
         <v>201</v>
       </c>
-      <c r="R2" s="108" t="s">
+      <c r="S2" s="108" t="s">
         <v>202</v>
       </c>
-      <c r="S2" s="108" t="s">
-        <v>203</v>
-      </c>
       <c r="T2" s="108" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="U2" s="108" t="s">
         <v>19</v>
@@ -1680,13 +1680,13 @@
         <v>20</v>
       </c>
       <c r="W2" s="108" t="s">
+        <v>204</v>
+      </c>
+      <c r="X2" s="108" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="108" t="s">
-        <v>22</v>
-      </c>
       <c r="Y2" s="108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="Z2" s="108" t="s">
         <v>9</v>
@@ -1698,10 +1698,10 @@
         <v>11</v>
       </c>
       <c r="AC2" s="108" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD2" s="108" t="s">
         <v>191</v>
-      </c>
-      <c r="AD2" s="108" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:156" ht="20" x14ac:dyDescent="0.2">
@@ -1709,10 +1709,10 @@
         <v>4</v>
       </c>
       <c r="F3" s="108" t="s">
+        <v>197</v>
+      </c>
+      <c r="G3" s="108" t="s">
         <v>198</v>
-      </c>
-      <c r="G3" s="108" t="s">
-        <v>199</v>
       </c>
       <c r="H3" s="108" t="s">
         <v>5</v>
@@ -2008,13 +2008,13 @@
         <v>2017</v>
       </c>
       <c r="B5" s="109" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="109" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="109" t="s">
+      <c r="D5" s="109" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="109" t="s">
-        <v>25</v>
       </c>
       <c r="E5" s="109"/>
       <c r="F5" s="109" t="s">
@@ -2186,13 +2186,13 @@
         <v>2022</v>
       </c>
       <c r="B6" s="109" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="D6" s="109" t="s">
         <v>27</v>
-      </c>
-      <c r="D6" s="109" t="s">
-        <v>28</v>
       </c>
       <c r="E6" s="109"/>
       <c r="F6" s="109" t="s">
@@ -2366,13 +2366,13 @@
         <v>2012</v>
       </c>
       <c r="B7" s="109" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="109" t="s">
+      <c r="D7" s="109" t="s">
         <v>30</v>
-      </c>
-      <c r="D7" s="109" t="s">
-        <v>31</v>
       </c>
       <c r="E7" s="109"/>
       <c r="F7" s="109"/>
@@ -2544,13 +2544,13 @@
         <v>2014</v>
       </c>
       <c r="B8" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="109" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="109" t="s">
         <v>32</v>
-      </c>
-      <c r="D8" s="109" t="s">
-        <v>33</v>
       </c>
       <c r="E8" s="109"/>
       <c r="F8" s="109"/>
@@ -2724,13 +2724,13 @@
         <v>2018</v>
       </c>
       <c r="B9" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="109" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="109" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" s="109" t="s">
-        <v>35</v>
       </c>
       <c r="E9" s="109"/>
       <c r="F9" s="109" t="s">
@@ -2906,13 +2906,13 @@
         <v>2022</v>
       </c>
       <c r="B10" s="109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="109" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="110" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10" s="109"/>
       <c r="F10" s="109" t="s">
@@ -3090,13 +3090,13 @@
         <v>2019</v>
       </c>
       <c r="B11" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" s="109" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="109" t="s">
         <v>37</v>
-      </c>
-      <c r="D11" s="109" t="s">
-        <v>38</v>
       </c>
       <c r="E11" s="109"/>
       <c r="F11" s="109" t="s">
@@ -3274,13 +3274,13 @@
         <v>2020</v>
       </c>
       <c r="B12" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" s="109" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D12" s="109" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E12" s="109"/>
       <c r="F12" s="109"/>
@@ -3452,13 +3452,13 @@
         <v>2020</v>
       </c>
       <c r="B13" s="109" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="109" t="s">
+      <c r="D13" s="109" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="109" t="s">
-        <v>42</v>
       </c>
       <c r="E13" s="109"/>
       <c r="F13" s="109"/>
@@ -3630,13 +3630,13 @@
         <v>2022</v>
       </c>
       <c r="B14" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="109" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D14" s="111" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="109"/>
       <c r="F14" s="109"/>
@@ -3810,13 +3810,13 @@
         <v>2010</v>
       </c>
       <c r="B15" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="109" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D15" s="109" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="109"/>
       <c r="F15" s="109"/>
@@ -3984,13 +3984,13 @@
         <v>2009</v>
       </c>
       <c r="B16" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="109" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="109" t="s">
         <v>45</v>
-      </c>
-      <c r="D16" s="109" t="s">
-        <v>46</v>
       </c>
       <c r="E16" s="109"/>
       <c r="F16" s="109"/>
@@ -4160,13 +4160,13 @@
         <v>2013</v>
       </c>
       <c r="B17" s="109" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="109" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="109" t="s">
+      <c r="D17" s="109" t="s">
         <v>48</v>
-      </c>
-      <c r="D17" s="109" t="s">
-        <v>49</v>
       </c>
       <c r="E17" s="109"/>
       <c r="F17" s="109"/>
@@ -4334,13 +4334,13 @@
         <v>2020</v>
       </c>
       <c r="B18" s="109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" s="109" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="109" t="s">
         <v>50</v>
-      </c>
-      <c r="D18" s="109" t="s">
-        <v>51</v>
       </c>
       <c r="E18" s="109"/>
       <c r="F18" s="109" t="s">
@@ -4520,13 +4520,13 @@
         <v>2018</v>
       </c>
       <c r="B19" s="109" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="109" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="109" t="s">
+      <c r="D19" s="109" t="s">
         <v>53</v>
-      </c>
-      <c r="D19" s="109" t="s">
-        <v>54</v>
       </c>
       <c r="E19" s="109" t="s">
         <v>3</v>
@@ -4698,13 +4698,13 @@
         <v>2019</v>
       </c>
       <c r="B20" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C20" s="109" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" s="109" t="s">
         <v>55</v>
-      </c>
-      <c r="D20" s="109" t="s">
-        <v>56</v>
       </c>
       <c r="E20" s="109" t="s">
         <v>3</v>
@@ -4882,13 +4882,13 @@
         <v>2016</v>
       </c>
       <c r="B21" s="109" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="109" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="109" t="s">
         <v>57</v>
-      </c>
-      <c r="D21" s="109" t="s">
-        <v>58</v>
       </c>
       <c r="E21" s="109" t="s">
         <v>3</v>
@@ -5060,13 +5060,13 @@
         <v>2017</v>
       </c>
       <c r="B22" s="109" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="109" t="s">
+      <c r="D22" s="109" t="s">
         <v>60</v>
-      </c>
-      <c r="D22" s="109" t="s">
-        <v>61</v>
       </c>
       <c r="E22" s="109" t="s">
         <v>3</v>
@@ -5232,13 +5232,13 @@
         <v>2019</v>
       </c>
       <c r="B23" s="109" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="109" t="s">
         <v>62</v>
       </c>
-      <c r="C23" s="109" t="s">
+      <c r="D23" s="109" t="s">
         <v>63</v>
-      </c>
-      <c r="D23" s="109" t="s">
-        <v>64</v>
       </c>
       <c r="E23" s="109"/>
       <c r="F23" s="109"/>
@@ -5406,13 +5406,13 @@
         <v>2021</v>
       </c>
       <c r="B24" s="109" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="109" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="109" t="s">
+      <c r="D24" s="109" t="s">
         <v>66</v>
-      </c>
-      <c r="D24" s="109" t="s">
-        <v>67</v>
       </c>
       <c r="E24" s="109"/>
       <c r="F24" s="109"/>
@@ -5578,13 +5578,13 @@
         <v>2018</v>
       </c>
       <c r="B25" s="109" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="109" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="109" t="s">
+      <c r="D25" s="109" t="s">
         <v>69</v>
-      </c>
-      <c r="D25" s="109" t="s">
-        <v>70</v>
       </c>
       <c r="E25" s="109" t="s">
         <v>3</v>
@@ -5752,13 +5752,13 @@
         <v>2019</v>
       </c>
       <c r="B26" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C26" s="109" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="109" t="s">
         <v>71</v>
-      </c>
-      <c r="D26" s="109" t="s">
-        <v>72</v>
       </c>
       <c r="E26" s="109"/>
       <c r="F26" s="109"/>
@@ -5924,13 +5924,13 @@
         <v>2021</v>
       </c>
       <c r="B27" s="109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="109" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" s="109" t="s">
         <v>73</v>
-      </c>
-      <c r="D27" s="109" t="s">
-        <v>74</v>
       </c>
       <c r="E27" s="109"/>
       <c r="F27" s="109" t="s">
@@ -6102,13 +6102,13 @@
         <v>2020</v>
       </c>
       <c r="B28" s="109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="109" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" s="109" t="s">
         <v>75</v>
-      </c>
-      <c r="D28" s="109" t="s">
-        <v>76</v>
       </c>
       <c r="E28" s="109" t="s">
         <v>3</v>
@@ -6280,13 +6280,13 @@
         <v>2019</v>
       </c>
       <c r="B29" s="109" t="s">
+        <v>76</v>
+      </c>
+      <c r="C29" s="109" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="109" t="s">
+      <c r="D29" s="109" t="s">
         <v>78</v>
-      </c>
-      <c r="D29" s="109" t="s">
-        <v>79</v>
       </c>
       <c r="E29" s="109" t="s">
         <v>3</v>
@@ -6458,13 +6458,13 @@
         <v>2020</v>
       </c>
       <c r="B30" s="109" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" s="109" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="109" t="s">
         <v>80</v>
-      </c>
-      <c r="C30" s="109" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="109" t="s">
-        <v>81</v>
       </c>
       <c r="E30" s="109"/>
       <c r="F30" s="109"/>
@@ -6638,13 +6638,13 @@
         <v>2018</v>
       </c>
       <c r="B31" s="109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="109" t="s">
+        <v>81</v>
+      </c>
+      <c r="D31" s="109" t="s">
         <v>82</v>
-      </c>
-      <c r="D31" s="109" t="s">
-        <v>83</v>
       </c>
       <c r="E31" s="109"/>
       <c r="F31" s="109" t="s">
@@ -6820,13 +6820,13 @@
         <v>2022</v>
       </c>
       <c r="B32" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="109" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="109" t="s">
         <v>84</v>
-      </c>
-      <c r="D32" s="109" t="s">
-        <v>85</v>
       </c>
       <c r="E32" s="109"/>
       <c r="F32" s="109" t="s">
@@ -6998,13 +6998,13 @@
         <v>2020</v>
       </c>
       <c r="B33" s="109" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="109" t="s">
         <v>86</v>
       </c>
-      <c r="C33" s="109" t="s">
+      <c r="D33" s="109" t="s">
         <v>87</v>
-      </c>
-      <c r="D33" s="109" t="s">
-        <v>88</v>
       </c>
       <c r="E33" s="109"/>
       <c r="F33" s="109"/>
@@ -7174,13 +7174,13 @@
         <v>2019</v>
       </c>
       <c r="B34" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="109" t="s">
         <v>89</v>
-      </c>
-      <c r="D34" s="109" t="s">
-        <v>90</v>
       </c>
       <c r="E34" s="109"/>
       <c r="F34" s="109"/>
@@ -7346,13 +7346,13 @@
         <v>2018</v>
       </c>
       <c r="B35" s="109" t="s">
+        <v>90</v>
+      </c>
+      <c r="C35" s="109" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="109" t="s">
+      <c r="D35" s="109" t="s">
         <v>92</v>
-      </c>
-      <c r="D35" s="109" t="s">
-        <v>93</v>
       </c>
       <c r="E35" s="109"/>
       <c r="F35" s="109"/>
@@ -7520,13 +7520,13 @@
         <v>2022</v>
       </c>
       <c r="B36" s="109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" s="109" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" s="109" t="s">
         <v>94</v>
-      </c>
-      <c r="D36" s="109" t="s">
-        <v>95</v>
       </c>
       <c r="E36" s="109"/>
       <c r="F36" s="109"/>
@@ -7694,13 +7694,13 @@
         <v>2019</v>
       </c>
       <c r="B37" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C37" s="109" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="109" t="s">
         <v>89</v>
-      </c>
-      <c r="D37" s="109" t="s">
-        <v>90</v>
       </c>
       <c r="E37" s="109"/>
       <c r="F37" s="109"/>
@@ -7868,13 +7868,13 @@
         <v>2020</v>
       </c>
       <c r="B38" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="109" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="109" t="s">
         <v>96</v>
-      </c>
-      <c r="D38" s="109" t="s">
-        <v>97</v>
       </c>
       <c r="E38" s="109"/>
       <c r="F38" s="109"/>
@@ -8042,13 +8042,13 @@
         <v>2020</v>
       </c>
       <c r="B39" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="109" t="s">
+        <v>97</v>
+      </c>
+      <c r="D39" s="109" t="s">
         <v>98</v>
-      </c>
-      <c r="D39" s="109" t="s">
-        <v>99</v>
       </c>
       <c r="E39" s="109"/>
       <c r="F39" s="109"/>
@@ -8212,13 +8212,13 @@
         <v>2018</v>
       </c>
       <c r="B40" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" s="109" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="109" t="s">
         <v>100</v>
-      </c>
-      <c r="D40" s="109" t="s">
-        <v>101</v>
       </c>
       <c r="E40" s="109"/>
       <c r="F40" s="109" t="s">
@@ -8382,13 +8382,13 @@
         <v>2022</v>
       </c>
       <c r="B41" s="109" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="109" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="109" t="s">
         <v>102</v>
-      </c>
-      <c r="D41" s="109" t="s">
-        <v>103</v>
       </c>
       <c r="E41" s="109"/>
       <c r="F41" s="109" t="s">
@@ -8556,13 +8556,13 @@
         <v>2017</v>
       </c>
       <c r="B42" s="109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C42" s="109" t="s">
+        <v>103</v>
+      </c>
+      <c r="D42" s="109" t="s">
         <v>104</v>
-      </c>
-      <c r="D42" s="109" t="s">
-        <v>105</v>
       </c>
       <c r="E42" s="109"/>
       <c r="F42" s="109"/>
@@ -8730,13 +8730,13 @@
         <v>2020</v>
       </c>
       <c r="B43" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C43" s="109" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" s="109" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E43" s="109"/>
       <c r="F43" s="109"/>
@@ -8900,13 +8900,13 @@
         <v>2019</v>
       </c>
       <c r="B44" s="109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" s="109" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" s="109" t="s">
         <v>107</v>
-      </c>
-      <c r="D44" s="109" t="s">
-        <v>108</v>
       </c>
       <c r="E44" s="109"/>
       <c r="F44" s="109"/>
@@ -9074,13 +9074,13 @@
         <v>2021</v>
       </c>
       <c r="B45" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C45" s="109" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" s="109" t="s">
         <v>109</v>
-      </c>
-      <c r="D45" s="109" t="s">
-        <v>110</v>
       </c>
       <c r="E45" s="109"/>
       <c r="F45" s="109" t="s">
@@ -9250,13 +9250,13 @@
         <v>2019</v>
       </c>
       <c r="B46" s="109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" s="109" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="109" t="s">
         <v>111</v>
-      </c>
-      <c r="D46" s="109" t="s">
-        <v>112</v>
       </c>
       <c r="E46" s="109" t="s">
         <v>3</v>
@@ -9428,13 +9428,13 @@
         <v>2019</v>
       </c>
       <c r="B47" s="109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C47" s="109" t="s">
+        <v>112</v>
+      </c>
+      <c r="D47" s="109" t="s">
         <v>113</v>
-      </c>
-      <c r="D47" s="109" t="s">
-        <v>114</v>
       </c>
       <c r="E47" s="109" t="s">
         <v>3</v>
@@ -9606,13 +9606,13 @@
         <v>2019</v>
       </c>
       <c r="B48" s="109" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C48" s="109" t="s">
+        <v>114</v>
+      </c>
+      <c r="D48" s="109" t="s">
         <v>115</v>
-      </c>
-      <c r="D48" s="109" t="s">
-        <v>116</v>
       </c>
       <c r="E48" s="109" t="s">
         <v>3</v>
@@ -9780,13 +9780,13 @@
         <v>2019</v>
       </c>
       <c r="B49" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C49" s="109" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D49" s="109" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E49" s="109"/>
       <c r="F49" s="109" t="s">
@@ -9954,13 +9954,13 @@
         <v>2020</v>
       </c>
       <c r="B50" s="109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C50" s="109" t="s">
+        <v>117</v>
+      </c>
+      <c r="D50" s="109" t="s">
         <v>118</v>
-      </c>
-      <c r="D50" s="109" t="s">
-        <v>119</v>
       </c>
       <c r="E50" s="109"/>
       <c r="F50" s="109" t="s">
@@ -10128,13 +10128,13 @@
         <v>2019</v>
       </c>
       <c r="B51" s="109" t="s">
+        <v>119</v>
+      </c>
+      <c r="C51" s="109" t="s">
         <v>120</v>
       </c>
-      <c r="C51" s="109" t="s">
+      <c r="D51" s="109" t="s">
         <v>121</v>
-      </c>
-      <c r="D51" s="109" t="s">
-        <v>122</v>
       </c>
       <c r="E51" s="109"/>
       <c r="F51" s="109"/>
@@ -10298,13 +10298,13 @@
         <v>2022</v>
       </c>
       <c r="B52" s="109" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="D52" s="109" t="s">
         <v>123</v>
-      </c>
-      <c r="D52" s="109" t="s">
-        <v>124</v>
       </c>
       <c r="E52" s="109"/>
       <c r="F52" s="109" t="s">
@@ -10476,13 +10476,13 @@
         <v>2022</v>
       </c>
       <c r="B53" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C53" s="109" t="s">
+        <v>124</v>
+      </c>
+      <c r="D53" s="109" t="s">
         <v>125</v>
-      </c>
-      <c r="D53" s="109" t="s">
-        <v>126</v>
       </c>
       <c r="E53" s="109"/>
       <c r="F53" s="109" t="s">
@@ -10650,13 +10650,13 @@
         <v>2020</v>
       </c>
       <c r="B54" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C54" s="109" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D54" s="109" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E54" s="109"/>
       <c r="F54" s="109"/>
@@ -10818,13 +10818,13 @@
         <v>2019</v>
       </c>
       <c r="B55" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C55" s="109" t="s">
+        <v>127</v>
+      </c>
+      <c r="D55" s="109" t="s">
         <v>128</v>
-      </c>
-      <c r="D55" s="109" t="s">
-        <v>129</v>
       </c>
       <c r="E55" s="109"/>
       <c r="F55" s="109"/>
@@ -10986,13 +10986,13 @@
         <v>2022</v>
       </c>
       <c r="B56" s="109" t="s">
+        <v>129</v>
+      </c>
+      <c r="C56" s="109" t="s">
         <v>130</v>
       </c>
-      <c r="C56" s="109" t="s">
+      <c r="D56" s="113" t="s">
         <v>131</v>
-      </c>
-      <c r="D56" s="113" t="s">
-        <v>132</v>
       </c>
       <c r="E56" s="109"/>
       <c r="F56" s="109"/>
@@ -11156,13 +11156,13 @@
         <v>2021</v>
       </c>
       <c r="B57" s="109" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C57" s="109" t="s">
+        <v>132</v>
+      </c>
+      <c r="D57" s="109" t="s">
         <v>133</v>
-      </c>
-      <c r="D57" s="109" t="s">
-        <v>134</v>
       </c>
       <c r="E57" s="109"/>
       <c r="F57" s="109"/>
@@ -11330,13 +11330,13 @@
         <v>2020</v>
       </c>
       <c r="B58" s="109" t="s">
+        <v>134</v>
+      </c>
+      <c r="C58" s="109" t="s">
         <v>135</v>
       </c>
-      <c r="C58" s="109" t="s">
+      <c r="D58" s="109" t="s">
         <v>136</v>
-      </c>
-      <c r="D58" s="109" t="s">
-        <v>137</v>
       </c>
       <c r="E58" s="109"/>
       <c r="F58" s="109"/>
@@ -11502,13 +11502,13 @@
         <v>2020</v>
       </c>
       <c r="B59" s="109" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C59" s="109" t="s">
+        <v>137</v>
+      </c>
+      <c r="D59" s="109" t="s">
         <v>138</v>
-      </c>
-      <c r="D59" s="109" t="s">
-        <v>139</v>
       </c>
       <c r="E59" s="109"/>
       <c r="F59" s="109" t="s">
@@ -11678,13 +11678,13 @@
         <v>2011</v>
       </c>
       <c r="B60" s="109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C60" s="109" t="s">
+        <v>139</v>
+      </c>
+      <c r="D60" s="109" t="s">
         <v>140</v>
-      </c>
-      <c r="D60" s="109" t="s">
-        <v>141</v>
       </c>
       <c r="E60" s="109"/>
       <c r="F60" s="109"/>
@@ -11848,13 +11848,13 @@
         <v>2021</v>
       </c>
       <c r="B61" s="109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C61" s="109" t="s">
+        <v>141</v>
+      </c>
+      <c r="D61" s="109" t="s">
         <v>142</v>
-      </c>
-      <c r="D61" s="109" t="s">
-        <v>143</v>
       </c>
       <c r="E61" s="109"/>
       <c r="F61" s="109"/>
@@ -12014,13 +12014,13 @@
         <v>2017</v>
       </c>
       <c r="B62" s="109" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" s="109" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" s="109" t="s">
         <v>144</v>
-      </c>
-      <c r="D62" s="109" t="s">
-        <v>145</v>
       </c>
       <c r="E62" s="109"/>
       <c r="F62" s="109"/>
@@ -12182,13 +12182,13 @@
         <v>2015</v>
       </c>
       <c r="B63" s="109" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="109" t="s">
         <v>146</v>
       </c>
-      <c r="C63" s="109" t="s">
+      <c r="D63" s="109" t="s">
         <v>147</v>
-      </c>
-      <c r="D63" s="109" t="s">
-        <v>148</v>
       </c>
       <c r="E63" s="109"/>
       <c r="F63" s="109"/>
@@ -12358,13 +12358,13 @@
         <v>2013</v>
       </c>
       <c r="B64" s="109" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C64" s="109" t="s">
+        <v>148</v>
+      </c>
+      <c r="D64" s="109" t="s">
         <v>149</v>
-      </c>
-      <c r="D64" s="109" t="s">
-        <v>150</v>
       </c>
       <c r="E64" s="109"/>
       <c r="F64" s="109"/>
@@ -12530,13 +12530,13 @@
         <v>2017</v>
       </c>
       <c r="B65" s="109" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="109" t="s">
+        <v>150</v>
+      </c>
+      <c r="D65" s="109" t="s">
         <v>151</v>
-      </c>
-      <c r="D65" s="109" t="s">
-        <v>152</v>
       </c>
       <c r="E65" s="109"/>
       <c r="F65" s="109"/>
@@ -12696,13 +12696,13 @@
         <v>2019</v>
       </c>
       <c r="B66" s="109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C66" s="109" t="s">
+        <v>152</v>
+      </c>
+      <c r="D66" s="109" t="s">
         <v>153</v>
-      </c>
-      <c r="D66" s="109" t="s">
-        <v>154</v>
       </c>
       <c r="E66" s="109"/>
       <c r="F66" s="109"/>
@@ -12866,13 +12866,13 @@
         <v>2018</v>
       </c>
       <c r="B67" s="109" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="109" t="s">
         <v>155</v>
       </c>
-      <c r="C67" s="109" t="s">
+      <c r="D67" s="109" t="s">
         <v>156</v>
-      </c>
-      <c r="D67" s="109" t="s">
-        <v>157</v>
       </c>
       <c r="E67" s="109"/>
       <c r="F67" s="109"/>
@@ -13034,13 +13034,13 @@
         <v>2017</v>
       </c>
       <c r="B68" s="109" t="s">
+        <v>157</v>
+      </c>
+      <c r="C68" s="109" t="s">
         <v>158</v>
       </c>
-      <c r="C68" s="109" t="s">
+      <c r="D68" s="109" t="s">
         <v>159</v>
-      </c>
-      <c r="D68" s="109" t="s">
-        <v>160</v>
       </c>
       <c r="E68" s="109"/>
       <c r="F68" s="109"/>
@@ -13208,13 +13208,13 @@
         <v>2019</v>
       </c>
       <c r="B69" s="109" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C69" s="109" t="s">
+        <v>160</v>
+      </c>
+      <c r="D69" s="109" t="s">
         <v>161</v>
-      </c>
-      <c r="D69" s="109" t="s">
-        <v>162</v>
       </c>
       <c r="E69" s="109"/>
       <c r="F69" s="109"/>
@@ -13374,13 +13374,13 @@
         <v>2021</v>
       </c>
       <c r="B70" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C70" s="109" t="s">
+        <v>162</v>
+      </c>
+      <c r="D70" s="109" t="s">
         <v>163</v>
-      </c>
-      <c r="D70" s="109" t="s">
-        <v>164</v>
       </c>
       <c r="E70" s="109"/>
       <c r="F70" s="109"/>
@@ -13542,13 +13542,13 @@
         <v>2022</v>
       </c>
       <c r="B71" s="109" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C71" s="109" t="s">
+        <v>164</v>
+      </c>
+      <c r="D71" s="109" t="s">
         <v>165</v>
-      </c>
-      <c r="D71" s="109" t="s">
-        <v>166</v>
       </c>
       <c r="E71" s="109"/>
       <c r="F71" s="109"/>
@@ -13710,13 +13710,13 @@
         <v>2019</v>
       </c>
       <c r="B72" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C72" s="109" t="s">
+        <v>166</v>
+      </c>
+      <c r="D72" s="109" t="s">
         <v>167</v>
-      </c>
-      <c r="D72" s="109" t="s">
-        <v>168</v>
       </c>
       <c r="E72" s="109"/>
       <c r="F72" s="109"/>
@@ -13878,13 +13878,13 @@
         <v>2017</v>
       </c>
       <c r="B73" s="109" t="s">
+        <v>168</v>
+      </c>
+      <c r="C73" s="109" t="s">
         <v>169</v>
       </c>
-      <c r="C73" s="109" t="s">
+      <c r="D73" s="109" t="s">
         <v>170</v>
-      </c>
-      <c r="D73" s="109" t="s">
-        <v>171</v>
       </c>
       <c r="E73" s="109"/>
       <c r="F73" s="109"/>
@@ -14046,13 +14046,13 @@
         <v>2021</v>
       </c>
       <c r="B74" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C74" s="109" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="109" t="s">
         <v>172</v>
-      </c>
-      <c r="D74" s="109" t="s">
-        <v>173</v>
       </c>
       <c r="E74" s="109"/>
       <c r="F74" s="109"/>
@@ -14220,13 +14220,13 @@
         <v>2021</v>
       </c>
       <c r="B75" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C75" s="109" t="s">
+        <v>173</v>
+      </c>
+      <c r="D75" s="114" t="s">
         <v>174</v>
-      </c>
-      <c r="D75" s="114" t="s">
-        <v>175</v>
       </c>
       <c r="E75" s="109"/>
       <c r="F75" s="109"/>
@@ -14400,13 +14400,13 @@
         <v>2021</v>
       </c>
       <c r="B76" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C76" s="109" t="s">
+        <v>175</v>
+      </c>
+      <c r="D76" s="109" t="s">
         <v>176</v>
-      </c>
-      <c r="D76" s="109" t="s">
-        <v>177</v>
       </c>
       <c r="E76" s="109"/>
       <c r="F76" s="109"/>
@@ -14570,13 +14570,13 @@
         <v>2021</v>
       </c>
       <c r="B77" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C77" s="109" t="s">
+        <v>177</v>
+      </c>
+      <c r="D77" s="109" t="s">
         <v>178</v>
-      </c>
-      <c r="D77" s="109" t="s">
-        <v>179</v>
       </c>
       <c r="E77" s="109"/>
       <c r="F77" s="109"/>
@@ -14740,13 +14740,13 @@
         <v>2021</v>
       </c>
       <c r="B78" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C78" s="109" t="s">
+        <v>179</v>
+      </c>
+      <c r="D78" s="109" t="s">
         <v>180</v>
-      </c>
-      <c r="D78" s="109" t="s">
-        <v>181</v>
       </c>
       <c r="E78" s="109"/>
       <c r="F78" s="109" t="s">
@@ -14914,13 +14914,13 @@
         <v>2021</v>
       </c>
       <c r="B79" s="109" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C79" s="109" t="s">
+        <v>181</v>
+      </c>
+      <c r="D79" s="109" t="s">
         <v>182</v>
-      </c>
-      <c r="D79" s="109" t="s">
-        <v>183</v>
       </c>
       <c r="E79" s="109"/>
       <c r="F79" s="109"/>
@@ -15088,13 +15088,13 @@
         <v>2021</v>
       </c>
       <c r="B80" s="109" t="s">
+        <v>183</v>
+      </c>
+      <c r="C80" s="109" t="s">
         <v>184</v>
       </c>
-      <c r="C80" s="109" t="s">
+      <c r="D80" s="109" t="s">
         <v>185</v>
-      </c>
-      <c r="D80" s="109" t="s">
-        <v>186</v>
       </c>
       <c r="E80" s="109"/>
       <c r="F80" s="109" t="s">

</xml_diff>